<commit_message>
updating raw data and git ignore files
</commit_message>
<xml_diff>
--- a/raw/growth_loss.xlsx
+++ b/raw/growth_loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Aerial Data\Area E drone data\Dana\QGIS\classified_GEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81172B87-BB42-47FB-9272-8FBEC4566693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A207BB3-F467-4717-82ED-D4578C7CD1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5724" yWindow="0" windowWidth="17280" windowHeight="10104" firstSheet="3" activeTab="7" xr2:uid="{0B7B4DF4-3F14-4B08-8CC2-D6EC6A4F628B}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="10308" windowHeight="12768" firstSheet="3" activeTab="6" xr2:uid="{0B7B4DF4-3F14-4B08-8CC2-D6EC6A4F628B}"/>
   </bookViews>
   <sheets>
     <sheet name="46-42" sheetId="1" r:id="rId1"/>
@@ -1060,10 +1060,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1084,13 +1087,13 @@
         <v>-3</v>
       </c>
       <c r="B2" s="1">
-        <v>876261</v>
+        <v>542247</v>
       </c>
       <c r="C2" s="1">
-        <v>8762.6100000299994</v>
+        <v>5422.4699999000004</v>
       </c>
       <c r="D2" s="1">
-        <v>0.876</v>
+        <v>0.54200000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1098,13 +1101,13 @@
         <v>-2</v>
       </c>
       <c r="B3" s="1">
-        <v>362960</v>
+        <v>349351</v>
       </c>
       <c r="C3" s="1">
-        <v>3629.6000000099998</v>
+        <v>3493.51</v>
       </c>
       <c r="D3" s="1">
-        <v>0.36299999999999999</v>
+        <v>0.34899999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1112,13 +1115,13 @@
         <v>-1</v>
       </c>
       <c r="B4" s="1">
-        <v>1577569</v>
+        <v>1046739</v>
       </c>
       <c r="C4" s="1">
-        <v>15775.69000006</v>
+        <v>10467.3899999</v>
       </c>
       <c r="D4" s="1">
-        <v>1.5780000000000001</v>
+        <v>1.0469999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1126,13 +1129,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>42216829</v>
+        <v>17042925</v>
       </c>
       <c r="C5" s="1">
-        <v>422168.29000149999</v>
+        <v>170429.2499998</v>
       </c>
       <c r="D5" s="1">
-        <v>42.216999999999999</v>
+        <v>17.042999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1140,13 +1143,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>356469</v>
+        <v>290615</v>
       </c>
       <c r="C6" s="1">
-        <v>3564.6900000099999</v>
+        <v>2906.15</v>
       </c>
       <c r="D6" s="1">
-        <v>0.35599999999999998</v>
+        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1154,13 +1157,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>788447</v>
+        <v>781153</v>
       </c>
       <c r="C7" s="1">
-        <v>7884.4700000299999</v>
+        <v>7811.5299999899999</v>
       </c>
       <c r="D7" s="1">
-        <v>0.78800000000000003</v>
+        <v>0.78100000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1168,13 +1171,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>956226</v>
+        <v>924255</v>
       </c>
       <c r="C8" s="1">
-        <v>9562.2600000300008</v>
+        <v>9242.5499999900003</v>
       </c>
       <c r="D8" s="1">
-        <v>0.95599999999999996</v>
+        <v>0.92400000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1186,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17556349-FFDD-46BC-B325-6C6B19623267}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,13 +1214,13 @@
         <v>-3</v>
       </c>
       <c r="B2" s="1">
-        <v>232278</v>
+        <v>208424</v>
       </c>
       <c r="C2" s="1">
-        <v>2322.7800000000002</v>
+        <v>2084.2399999999998</v>
       </c>
       <c r="D2" s="1">
-        <v>0.23200000000000001</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1225,13 +1228,13 @@
         <v>-2</v>
       </c>
       <c r="B3" s="1">
-        <v>347979</v>
+        <v>361215</v>
       </c>
       <c r="C3" s="1">
-        <v>3479.79</v>
+        <v>3612.15</v>
       </c>
       <c r="D3" s="1">
-        <v>0.34799999999999998</v>
+        <v>0.36099999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1239,13 +1242,13 @@
         <v>-1</v>
       </c>
       <c r="B4" s="1">
-        <v>884951</v>
+        <v>770714</v>
       </c>
       <c r="C4" s="1">
-        <v>8849.5099999899994</v>
+        <v>7707.1399999900004</v>
       </c>
       <c r="D4" s="1">
-        <v>0.88500000000000001</v>
+        <v>0.77100000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1253,13 +1256,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>33290273</v>
+        <v>17823870</v>
       </c>
       <c r="C5" s="1">
-        <v>332902.72999962</v>
+        <v>178238.69999980001</v>
       </c>
       <c r="D5" s="1">
-        <v>33.29</v>
+        <v>17.824000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1267,13 +1270,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>1392215</v>
+        <v>749324</v>
       </c>
       <c r="C6" s="1">
-        <v>13922.14999998</v>
+        <v>7493.2399999899999</v>
       </c>
       <c r="D6" s="1">
-        <v>1.3919999999999999</v>
+        <v>0.749</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1281,13 +1284,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>448338</v>
+        <v>427202</v>
       </c>
       <c r="C7" s="1">
-        <v>4483.3799999900002</v>
+        <v>4272.0200000000004</v>
       </c>
       <c r="D7" s="1">
-        <v>0.44800000000000001</v>
+        <v>0.42699999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1295,13 +1298,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>932479</v>
+        <v>636536</v>
       </c>
       <c r="C8" s="1">
-        <v>9324.7899999900001</v>
+        <v>6365.3599999899998</v>
       </c>
       <c r="D8" s="1">
-        <v>0.93200000000000005</v>
+        <v>0.63700000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1313,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E99D82F-3401-48EE-AB1B-A8EE1DD9DCD9}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>